<commit_message>
added motorcycle sales dataset
</commit_message>
<xml_diff>
--- a/Data Science Course/1. Programming/1. Excel/Motorcycle-Shop-Dataset.xlsx
+++ b/Data Science Course/1. Programming/1. Excel/Motorcycle-Shop-Dataset.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="9030" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="9030"/>
   </bookViews>
   <sheets>
     <sheet name="Copyright" sheetId="4" r:id="rId1"/>
@@ -1084,7 +1084,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S15"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
@@ -1190,7 +1190,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2743,7 +2743,7 @@
         <v>23</v>
       </c>
       <c r="D2">
-        <v>34100</v>
+        <v>26200</v>
       </c>
       <c r="E2">
         <v>0.89</v>
@@ -2760,7 +2760,7 @@
         <v>22</v>
       </c>
       <c r="D3">
-        <v>35400</v>
+        <v>21600</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -2777,7 +2777,7 @@
         <v>27</v>
       </c>
       <c r="D4">
-        <v>33400</v>
+        <v>18700</v>
       </c>
       <c r="E4">
         <v>0.74</v>
@@ -2794,7 +2794,7 @@
         <v>6</v>
       </c>
       <c r="D5">
-        <v>34400</v>
+        <v>37600</v>
       </c>
       <c r="E5">
         <v>0.97</v>
@@ -2811,7 +2811,7 @@
         <v>8</v>
       </c>
       <c r="D6">
-        <v>37100</v>
+        <v>31000</v>
       </c>
       <c r="E6">
         <v>0.93</v>
@@ -2828,7 +2828,7 @@
         <v>19</v>
       </c>
       <c r="D7">
-        <v>31100</v>
+        <v>35800</v>
       </c>
       <c r="E7">
         <v>0.91</v>
@@ -2845,7 +2845,7 @@
         <v>7</v>
       </c>
       <c r="D8">
-        <v>64100</v>
+        <v>39500</v>
       </c>
       <c r="E8">
         <v>0.88</v>
@@ -2862,7 +2862,7 @@
         <v>34</v>
       </c>
       <c r="D9">
-        <v>8900</v>
+        <v>9100</v>
       </c>
       <c r="E9">
         <v>0.49</v>
@@ -2879,7 +2879,7 @@
         <v>36</v>
       </c>
       <c r="D10">
-        <v>1800</v>
+        <v>2200</v>
       </c>
       <c r="E10">
         <v>0.44</v>
@@ -2896,7 +2896,7 @@
         <v>35</v>
       </c>
       <c r="D11">
-        <v>17300</v>
+        <v>18400</v>
       </c>
       <c r="E11">
         <v>0.77</v>
@@ -2913,7 +2913,7 @@
         <v>33</v>
       </c>
       <c r="D12">
-        <v>9700</v>
+        <v>11000</v>
       </c>
       <c r="E12">
         <v>0.56999999999999995</v>
@@ -2930,7 +2930,7 @@
         <v>37</v>
       </c>
       <c r="D13">
-        <v>3500</v>
+        <v>4100</v>
       </c>
       <c r="E13">
         <v>0.41</v>
@@ -2947,7 +2947,7 @@
         <v>29</v>
       </c>
       <c r="D14">
-        <v>2800</v>
+        <v>3100</v>
       </c>
       <c r="E14">
         <v>0.31</v>
@@ -2964,7 +2964,7 @@
         <v>26</v>
       </c>
       <c r="D15">
-        <v>4100</v>
+        <v>3500</v>
       </c>
       <c r="E15">
         <v>0.38</v>
@@ -2981,7 +2981,7 @@
         <v>28</v>
       </c>
       <c r="D16">
-        <v>36400</v>
+        <v>33900</v>
       </c>
       <c r="E16">
         <v>0.98</v>
@@ -2998,7 +2998,7 @@
         <v>12</v>
       </c>
       <c r="D17">
-        <v>27400</v>
+        <v>31500</v>
       </c>
       <c r="E17">
         <v>0.93</v>
@@ -3015,7 +3015,7 @@
         <v>11</v>
       </c>
       <c r="D18">
-        <v>7900</v>
+        <v>6100</v>
       </c>
       <c r="E18">
         <v>0.49</v>
@@ -3032,7 +3032,7 @@
         <v>25</v>
       </c>
       <c r="D19">
-        <v>4400</v>
+        <v>3800</v>
       </c>
       <c r="E19">
         <v>0.28999999999999998</v>
@@ -3049,7 +3049,7 @@
         <v>30</v>
       </c>
       <c r="D20">
-        <v>1000</v>
+        <v>1100</v>
       </c>
       <c r="E20">
         <v>0.12</v>
@@ -3066,7 +3066,7 @@
         <v>31</v>
       </c>
       <c r="D21">
-        <v>2900</v>
+        <v>3500</v>
       </c>
       <c r="E21">
         <v>0.28999999999999998</v>
@@ -3083,7 +3083,7 @@
         <v>24</v>
       </c>
       <c r="D22">
-        <v>23400</v>
+        <v>19000</v>
       </c>
       <c r="E22">
         <v>0.94</v>
@@ -3100,7 +3100,7 @@
         <v>20</v>
       </c>
       <c r="D23">
-        <v>3500</v>
+        <v>4600</v>
       </c>
       <c r="E23">
         <v>0.75</v>
@@ -3117,7 +3117,7 @@
         <v>15</v>
       </c>
       <c r="D24">
-        <v>1000</v>
+        <v>1400</v>
       </c>
       <c r="E24">
         <v>0.81</v>
@@ -3134,7 +3134,7 @@
         <v>16</v>
       </c>
       <c r="D25">
-        <v>5800</v>
+        <v>6700</v>
       </c>
       <c r="E25">
         <v>0.41</v>
@@ -3151,7 +3151,7 @@
         <v>18</v>
       </c>
       <c r="D26">
-        <v>20400</v>
+        <v>16000</v>
       </c>
       <c r="E26">
         <v>0.81</v>
@@ -3168,7 +3168,7 @@
         <v>14</v>
       </c>
       <c r="D27">
-        <v>5400</v>
+        <v>3400</v>
       </c>
       <c r="E27">
         <v>0.57999999999999996</v>
@@ -3185,7 +3185,7 @@
         <v>21</v>
       </c>
       <c r="D28">
-        <v>6600</v>
+        <v>12800</v>
       </c>
       <c r="E28">
         <v>0.28999999999999998</v>
@@ -3202,7 +3202,7 @@
         <v>32</v>
       </c>
       <c r="D29">
-        <v>800</v>
+        <v>3500</v>
       </c>
       <c r="E29">
         <v>0.39</v>
@@ -3219,7 +3219,7 @@
         <v>17</v>
       </c>
       <c r="D30">
-        <v>22200</v>
+        <v>31500</v>
       </c>
       <c r="E30">
         <v>0.99</v>

</xml_diff>